<commit_message>
xgboost initial set up
</commit_message>
<xml_diff>
--- a/available_profiles.xlsx
+++ b/available_profiles.xlsx
@@ -497,11 +497,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>338</v>
+        <v>259</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>Bob Williams</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -509,17 +509,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>£680-£1115</t>
+          <t>£409-£411</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -530,14 +530,10 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -545,21 +541,21 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>162</v>
+        <v>327</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -568,40 +564,36 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>£491-£913</t>
+          <t>£919-£1102</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Computer Science</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -609,33 +601,37 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>£301-£1565</t>
+          <t>£680-£1115</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -645,51 +641,47 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>224</v>
+        <v>337</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>John Williams</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>£722-£1914</t>
+          <t>£301-£1565</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Business</t>
-        </is>
-      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -699,7 +691,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
@@ -755,38 +747,42 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>430</v>
+        <v>249</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>£932-£1288</t>
+          <t>£693-£1053</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -799,21 +795,21 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Bob Smith</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -822,7 +818,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>£783-£1653</t>
+          <t>£491-£913</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -832,16 +828,16 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -849,35 +845,35 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>327</v>
+        <v>430</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>Jane Smith</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>£919-£1102</t>
+          <t>£932-£1288</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -887,21 +883,25 @@
       </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>249</v>
+        <v>174</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -909,7 +909,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -918,25 +918,21 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>£693-£1053</t>
+          <t>£783-£1653</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Computer Science</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -949,17 +945,17 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bob Williams</t>
+          <t>John Williams</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -967,17 +963,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>£409-£411</t>
+          <t>£722-£1914</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -988,10 +984,14 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Computer Science</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -999,17 +999,17 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>424</v>
+        <v>280</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1017,35 +1017,31 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>£747-£1274</t>
+          <t>£562-£1835</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -1053,7 +1049,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1105,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1126,62 +1122,62 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>£562-£1835</t>
+          <t>£332-£396</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>481</v>
+        <v>56</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bob Johnson</t>
+          <t>Bob Doe</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>£506-£762</t>
+          <t>£700-£1308</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1191,29 +1187,29 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Media</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>279</v>
+        <v>481</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1221,33 +1217,37 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>£332-£396</t>
+          <t>£506-£762</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1257,48 +1257,48 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>56</v>
+        <v>476</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Bob Doe</t>
+          <t>Bob Williams</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>£700-£1308</t>
+          <t>£974-£1569</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr"/>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>No</t>
@@ -1306,26 +1306,26 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>152</v>
+        <v>364</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Alice Smith</t>
+          <t>Alice Doe</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>£657-£1098</t>
+          <t>£480-£911</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1344,20 +1344,16 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -1365,21 +1361,21 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>63</v>
+        <v>424</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Alice Smith</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1388,7 +1384,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>£732-£1515</t>
+          <t>£747-£1274</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1398,15 +1394,15 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr"/>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>No</t>
@@ -1414,57 +1410,61 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>364</v>
+        <v>63</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Alice Doe</t>
+          <t>Alice Smith</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>£480-£911</t>
+          <t>£732-£1515</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Business</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1475,50 +1475,50 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>476</v>
+        <v>152</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bob Williams</t>
+          <t>Alice Smith</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>£974-£1569</t>
+          <t>£657-£1098</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Business</t>
-        </is>
-      </c>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1529,11 +1529,11 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>270</v>
+        <v>179</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>Bob Doe</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1546,12 +1546,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>£496-£1910</t>
+          <t>£967-£1996</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1577,45 +1577,53 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bob Johnson</t>
+          <t>Alice Smith</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>£662-£1471</t>
+          <t>£924-£1771</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr">
         <is>
           <t>Night</t>
@@ -1623,21 +1631,21 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>268</v>
+        <v>387</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Bob Doe</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1646,7 +1654,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>£397-£1988</t>
+          <t>£961-£1546</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1661,7 +1669,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Tech</t>
+          <t>Media</t>
         </is>
       </c>
       <c r="I24" t="inlineStr"/>
@@ -1673,13 +1681,13 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>387</v>
+        <v>318</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1687,21 +1695,21 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>£961-£1546</t>
+          <t>£596-£702</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1711,33 +1719,37 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Media</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>179</v>
+        <v>441</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Bob Doe</t>
+          <t>Alice Smith</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1746,44 +1758,44 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>£967-£1996</t>
+          <t>£331-£614</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>438</v>
+        <v>270</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1791,16 +1803,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>£831-£1862</t>
+          <t>£496-£1910</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1810,156 +1822,148 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>285</v>
+        <v>438</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Alice Smith</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>£924-£1771</t>
+          <t>£831-£1862</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>441</v>
+        <v>309</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Alice Smith</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>£331-£614</t>
+          <t>£662-£1471</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>120</v>
+        <v>494</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Alice Williams</t>
+          <t>Bob Doe</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>£916-£1859</t>
+          <t>£650-£1600</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1975,31 +1979,31 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>318</v>
+        <v>120</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>Alice Williams</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -2008,12 +2012,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>£596-£702</t>
+          <t>£916-£1859</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2023,37 +2027,37 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Media</t>
         </is>
       </c>
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>137</v>
+        <v>349</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Jane Williams</t>
+          <t>Alice Williams</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -2062,26 +2066,30 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>£981-£1295</t>
+          <t>£995-£1893</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>Business</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr"/>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr">
         <is>
           <t>Night</t>
@@ -2095,15 +2103,15 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>13</v>
+        <v>268</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>Bob Doe</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -2112,12 +2120,12 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>£397-£805</t>
+          <t>£397-£1988</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2145,15 +2153,15 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>349</v>
+        <v>258</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Alice Williams</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -2162,12 +2170,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>£995-£1893</t>
+          <t>£648-£792</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -2177,15 +2185,11 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Media</t>
         </is>
       </c>
       <c r="I34" t="inlineStr"/>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
           <t>Night</t>
@@ -2199,15 +2203,15 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>494</v>
+        <v>13</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Bob Doe</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -2216,12 +2220,12 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>£650-£1600</t>
+          <t>£397-£805</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -2231,18 +2235,14 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Media</t>
+          <t>Tech</t>
         </is>
       </c>
       <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -2253,7 +2253,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>258</v>
+        <v>36</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -2261,7 +2261,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -2270,25 +2270,25 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>£648-£792</t>
+          <t>£960-£1169</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>Media</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr"/>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr">
         <is>
@@ -2297,21 +2297,21 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>137</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Jane Williams</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>£960-£1169</t>
+          <t>£981-£1295</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2336,7 +2336,7 @@
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Business</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Rules Based to ship 16/01/2025
</commit_message>
<xml_diff>
--- a/available_profiles.xlsx
+++ b/available_profiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,15 +497,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -514,12 +514,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>£634-£1646</t>
+          <t>£397-£805</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -529,15 +529,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Media</t>
+          <t>Tech</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -545,21 +541,21 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -568,29 +564,29 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>£464-£1910</t>
+          <t>£960-£1169</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -601,11 +597,11 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>Bob Doe</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -618,7 +614,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>£748-£949</t>
+          <t>£700-£1308</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -633,25 +629,29 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Tech</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -659,21 +659,21 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>£694-£851</t>
+          <t>£732-£1515</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -683,14 +683,18 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Tech</t>
         </is>
       </c>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -701,37 +705,41 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Alice Williams</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>£751-£1401</t>
+          <t>£916-£1859</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
@@ -745,56 +753,52 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>Jane Williams</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>£615-£1095</t>
+          <t>£981-£1295</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -805,24 +809,24 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>45</v>
+        <v>152</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>Alice Smith</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>£963-£1604</t>
+          <t>£657-£1098</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -832,47 +836,51 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jane Doe</t>
+          <t>Bob Smith</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>£689-£1859</t>
+          <t>£491-£913</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -882,15 +890,15 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Media</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
@@ -899,21 +907,21 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>John Johnson</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -922,26 +930,26 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>£549-£673</t>
+          <t>£783-£1653</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -949,75 +957,75 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>John Johnson</t>
+          <t>Bob Doe</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>£737-£1603</t>
+          <t>£967-£1996</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr"/>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>122</v>
+        <v>189</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>John Johnson</t>
+          <t>Alice Doe</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1026,12 +1034,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>£894-£1776</t>
+          <t>£393-£558</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1042,7 +1050,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Business</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -1053,30 +1061,30 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>147</v>
+        <v>224</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>John Williams</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>£908-£1711</t>
+          <t>£722-£1914</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1086,11 +1094,15 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr">
         <is>
           <t>No</t>
@@ -1098,26 +1110,26 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>157</v>
+        <v>249</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bob Williams</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1126,24 +1138,28 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>£735-£746</t>
+          <t>£693-£1053</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1159,15 +1175,15 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>207</v>
+        <v>258</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bob Smith</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1176,66 +1192,62 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>£475-£1552</t>
+          <t>£648-£792</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>209</v>
+        <v>259</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Alice Williams</t>
+          <t>Bob Williams</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>£390-£1998</t>
+          <t>£409-£411</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1246,14 +1258,10 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -1261,17 +1269,17 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>224</v>
+        <v>268</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>John Williams</t>
+          <t>Bob Doe</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1279,12 +1287,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>£998-£1830</t>
+          <t>£397-£1988</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1294,38 +1302,38 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Business</t>
-        </is>
-      </c>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>256</v>
+        <v>270</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1334,12 +1342,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>£611-£681</t>
+          <t>£496-£1910</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1355,12 +1363,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1375,11 +1383,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Jane Johnson</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1388,26 +1396,26 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>£639-£681</t>
+          <t>£332-£396</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr">
         <is>
           <t>Night</t>
@@ -1421,50 +1429,46 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Alice Williams</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>£509-£1931</t>
+          <t>£562-£1835</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Business</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1475,15 +1479,15 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>Alice Smith</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1492,21 +1496,25 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>£921-£1859</t>
+          <t>£924-£1771</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -1519,56 +1527,48 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-08</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Alice Smith</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>£682-£708</t>
+          <t>£662-£1471</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Media</t>
-        </is>
-      </c>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -1579,11 +1579,11 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>393</v>
+        <v>318</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1591,17 +1591,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>£781-£1512</t>
+          <t>£596-£702</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1611,69 +1611,61 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Media</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>394</v>
+        <v>327</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>£990-£1711</t>
+          <t>£919-£1102</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
           <t>Night</t>
@@ -1681,51 +1673,47 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>396</v>
+        <v>337</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Alice Williams</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>£499-£760</t>
+          <t>£301-£1565</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -1735,21 +1723,21 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>412</v>
+        <v>338</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1758,24 +1746,28 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>£771-£1275</t>
+          <t>£680-£1115</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -1791,24 +1783,24 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>424</v>
+        <v>349</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Jane Johnson</t>
+          <t>Alice Williams</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>£675-£1285</t>
+          <t>£995-£1893</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1823,7 +1815,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Media</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="I27" t="inlineStr"/>
@@ -1839,17 +1831,17 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2024-09</t>
+          <t>2024-10</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>468</v>
+        <v>364</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Bob Doe</t>
+          <t>Alice Doe</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1857,35 +1849,31 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>£642-£1110</t>
+          <t>£480-£911</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -1893,52 +1881,52 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2024-10</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>469</v>
+        <v>387</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>John Johnson</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>£945-£1908</t>
+          <t>£961-£1546</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr"/>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -1949,42 +1937,42 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>477</v>
+        <v>388</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>£490-£1755</t>
+          <t>£432-£987</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Computer Science</t>
-        </is>
-      </c>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
@@ -1993,57 +1981,373 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2024-08</t>
+          <t>2024-09</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>484</v>
+        <v>424</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>John Smith</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>20</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>£747-£1274</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>2024-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>430</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>24</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>£932-£1288</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>2024-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>438</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Alice Johnson</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>18</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>£831-£1862</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>2024-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>441</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>Alice Smith</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="C34" t="n">
+        <v>24</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>£331-£614</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>2024-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>476</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Bob Williams</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>21</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>£974-£1569</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Night</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>2024-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>481</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Bob Johnson</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
         <v>23</v>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>£506-£762</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Night</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>2024-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>494</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Bob Doe</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>19</v>
+      </c>
+      <c r="D37" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>£382-£382</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>£650-£1600</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>2024-09</t>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Night</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>2024-08</t>
         </is>
       </c>
     </row>

</xml_diff>